<commit_message>
+ evaluate multiple target
</commit_message>
<xml_diff>
--- a/data/rough detection evaluation.xlsx
+++ b/data/rough detection evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\github\Socket_3Detection\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769F7371-979F-4DAB-9F8C-4F4A25F64B84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5746DB7-A841-45D5-B1F9-456D9EC5DA04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rough detection" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>dataset\iteration number</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>delta Dx, Dy, Dz</t>
+  </si>
+  <si>
+    <t>Socket</t>
+  </si>
+  <si>
+    <t>Plug</t>
   </si>
 </sst>
 </file>
@@ -90,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -100,6 +106,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1546,6 +1555,494 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'fine detection'!$B$2:$Z$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>791581.40359397698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>568037.02273807605</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>757170.0317392</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>725533.41389644297</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>843016.860306649</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>744905.60813658603</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>765667.81989947997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>713890.47754329199</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>741785.07029414899</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>544685.96085244499</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>720655.67184197204</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>737892.77921639802</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>768002.56736206799</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>794301.86031871801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>775901.92505946197</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>774379.28911221703</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>768241.27916546096</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>759983.57560704194</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>798893.68633358204</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>808361.12534580403</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>817618.25232239498</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>783102.51103498996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>812105.78632631502</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>803781.95372366905</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>825340.15761123796</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D7D2-4B15-B09A-261C0979EA62}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'fine detection'!$B$3:$Z$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>126509.094242701</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>121950.6016861</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>112273.32048179601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103277.90362216601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124229.745894012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>122283.071301663</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>121056.011059496</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>117689.82261991499</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>122260.63249664901</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>116804.66644046801</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>125627.05501353</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>122436.69959345199</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>108683.738790747</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>122980.73178032599</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>114740.681484259</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>117987.37328424399</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>118259.814930019</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>118345.43948623299</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>119386.35570907401</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>128898.030788448</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>126114.27682339201</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>123864.52329065499</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>130169.176358236</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>129858.616862346</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>129337.773451167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D7D2-4B15-B09A-261C0979EA62}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="802812336"/>
+        <c:axId val="802818896"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="802812336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="802818896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="802818896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="802812336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1626,6 +2123,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2305,6 +2842,509 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2727,6 +3767,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>293914</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>97971</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>217715</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>119743</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14F3FEEE-B6E6-4BA1-9E53-1E41FD480111}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3001,7 +4082,7 @@
   <dimension ref="A1:Z40"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="A2" sqref="A2:Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3016,34 +4097,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="1" t="s">
@@ -3865,11 +4946,9 @@
         <v>21972.342786266992</v>
       </c>
     </row>
-    <row r="11" spans="1:26"/>
     <row r="13" spans="1:26">
       <c r="S13" s="4"/>
     </row>
-    <row r="14" spans="1:26"/>
     <row r="15" spans="1:26">
       <c r="P15" t="s">
         <v>2</v>
@@ -3880,7 +4959,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="16:16"/>
     <row r="18" spans="16:16">
       <c r="P18" t="s">
         <v>4</v>
@@ -3904,14 +4982,256 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{818A5ED0-3732-4541-BC03-B4D94A89DBCE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:26">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="C1">
+        <v>20</v>
+      </c>
+      <c r="D1">
+        <v>30</v>
+      </c>
+      <c r="E1">
+        <v>40</v>
+      </c>
+      <c r="F1">
+        <v>50</v>
+      </c>
+      <c r="G1">
+        <v>60</v>
+      </c>
+      <c r="H1">
+        <v>70</v>
+      </c>
+      <c r="I1">
+        <v>80</v>
+      </c>
+      <c r="J1">
+        <v>90</v>
+      </c>
+      <c r="K1">
+        <v>100</v>
+      </c>
+      <c r="L1">
+        <v>110</v>
+      </c>
+      <c r="M1">
+        <v>120</v>
+      </c>
+      <c r="N1">
+        <v>130</v>
+      </c>
+      <c r="O1">
+        <v>140</v>
+      </c>
+      <c r="P1">
+        <v>150</v>
+      </c>
+      <c r="Q1">
+        <v>160</v>
+      </c>
+      <c r="R1">
+        <v>170</v>
+      </c>
+      <c r="S1">
+        <v>180</v>
+      </c>
+      <c r="T1">
+        <v>190</v>
+      </c>
+      <c r="U1">
+        <v>200</v>
+      </c>
+      <c r="V1">
+        <v>210</v>
+      </c>
+      <c r="W1">
+        <v>220</v>
+      </c>
+      <c r="X1">
+        <v>230</v>
+      </c>
+      <c r="Y1">
+        <v>240</v>
+      </c>
+      <c r="Z1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>791581.40359397698</v>
+      </c>
+      <c r="C2">
+        <v>568037.02273807605</v>
+      </c>
+      <c r="D2">
+        <v>757170.0317392</v>
+      </c>
+      <c r="E2">
+        <v>725533.41389644297</v>
+      </c>
+      <c r="F2">
+        <v>843016.860306649</v>
+      </c>
+      <c r="G2">
+        <v>744905.60813658603</v>
+      </c>
+      <c r="H2">
+        <v>765667.81989947997</v>
+      </c>
+      <c r="I2">
+        <v>713890.47754329199</v>
+      </c>
+      <c r="J2">
+        <v>741785.07029414899</v>
+      </c>
+      <c r="K2">
+        <v>544685.96085244499</v>
+      </c>
+      <c r="L2">
+        <v>720655.67184197204</v>
+      </c>
+      <c r="M2">
+        <v>737892.77921639802</v>
+      </c>
+      <c r="N2">
+        <v>768002.56736206799</v>
+      </c>
+      <c r="O2">
+        <v>794301.86031871801</v>
+      </c>
+      <c r="P2">
+        <v>775901.92505946197</v>
+      </c>
+      <c r="Q2">
+        <v>774379.28911221703</v>
+      </c>
+      <c r="R2">
+        <v>768241.27916546096</v>
+      </c>
+      <c r="S2">
+        <v>759983.57560704194</v>
+      </c>
+      <c r="T2">
+        <v>798893.68633358204</v>
+      </c>
+      <c r="U2">
+        <v>808361.12534580403</v>
+      </c>
+      <c r="V2">
+        <v>817618.25232239498</v>
+      </c>
+      <c r="W2">
+        <v>783102.51103498996</v>
+      </c>
+      <c r="X2">
+        <v>812105.78632631502</v>
+      </c>
+      <c r="Y2">
+        <v>803781.95372366905</v>
+      </c>
+      <c r="Z2">
+        <v>825340.15761123796</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>126509.094242701</v>
+      </c>
+      <c r="C3">
+        <v>121950.6016861</v>
+      </c>
+      <c r="D3">
+        <v>112273.32048179601</v>
+      </c>
+      <c r="E3">
+        <v>103277.90362216601</v>
+      </c>
+      <c r="F3">
+        <v>124229.745894012</v>
+      </c>
+      <c r="G3">
+        <v>122283.071301663</v>
+      </c>
+      <c r="H3">
+        <v>121056.011059496</v>
+      </c>
+      <c r="I3">
+        <v>117689.82261991499</v>
+      </c>
+      <c r="J3">
+        <v>122260.63249664901</v>
+      </c>
+      <c r="K3">
+        <v>116804.66644046801</v>
+      </c>
+      <c r="L3">
+        <v>125627.05501353</v>
+      </c>
+      <c r="M3">
+        <v>122436.69959345199</v>
+      </c>
+      <c r="N3">
+        <v>108683.738790747</v>
+      </c>
+      <c r="O3">
+        <v>122980.73178032599</v>
+      </c>
+      <c r="P3">
+        <v>114740.681484259</v>
+      </c>
+      <c r="Q3">
+        <v>117987.37328424399</v>
+      </c>
+      <c r="R3">
+        <v>118259.814930019</v>
+      </c>
+      <c r="S3">
+        <v>118345.43948623299</v>
+      </c>
+      <c r="T3">
+        <v>119386.35570907401</v>
+      </c>
+      <c r="U3">
+        <v>128898.030788448</v>
+      </c>
+      <c r="V3">
+        <v>126114.27682339201</v>
+      </c>
+      <c r="W3">
+        <v>123864.52329065499</v>
+      </c>
+      <c r="X3">
+        <v>130169.176358236</v>
+      </c>
+      <c r="Y3">
+        <v>129858.616862346</v>
+      </c>
+      <c r="Z3">
+        <v>129337.773451167</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>